<commit_message>
can get required data using HTTP requests
</commit_message>
<xml_diff>
--- a/database/testOld.xlsx
+++ b/database/testOld.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Desktop\code\gh-p\qgrs\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B15696-D78D-4A7F-8960-361C505EC227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6DFD2E-C099-4FCC-855D-B538020CD4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18780" yWindow="780" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19680" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testOld" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Lnc/ CircRNA name</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>12, 12</t>
-  </si>
-  <si>
-    <t>2, 2</t>
   </si>
   <si>
     <t>0, 0</t>
@@ -558,7 +555,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,108 +603,108 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +718,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -769,7 +766,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -778,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -799,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -808,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -820,7 +817,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -838,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -850,7 +847,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -868,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -880,7 +877,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -898,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -910,7 +907,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
@@ -928,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -940,7 +937,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
@@ -958,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -970,7 +967,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -988,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1000,7 +997,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -1018,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1030,7 +1027,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -1048,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1060,7 +1057,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -1078,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1090,7 +1087,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1108,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1120,7 +1117,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
@@ -1138,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1150,7 +1147,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
@@ -1168,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1180,7 +1177,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
@@ -1198,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1210,7 +1207,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -1228,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1240,7 +1237,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
@@ -1258,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1270,7 +1267,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3">
         <v>3</v>
@@ -1288,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>

</xml_diff>